<commit_message>
updates to parser project, getting there
</commit_message>
<xml_diff>
--- a/ACT-IAC_Events-02.27.23.xlsx
+++ b/ACT-IAC_Events-02.27.23.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorcas/Development/python_scraper_parser_projects/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339A0E0A-3384-1540-A4FF-CD14D0088C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="26680" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Events_Calendar" sheetId="1" r:id="rId1"/>
-    <sheet name="Projects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>Event_Type</t>
   </si>
@@ -179,19 +172,19 @@
     <t>Emerging Technology and Innovation are needed by government from both large and small businesses.</t>
   </si>
   <si>
-    <t>Join the ACT-IAC Acquisition COI member meeting featuring guest speaker Elizabeth (Liz) Chirico who leads the Acquisition Innovation through Technology team in the Office of the Deputy Assistant Secretary of the Army (Procurement) (ODASA(P).</t>
+    <t>Join the ACT-IAC Acquisition COI member meeting featuring guest speakers Elizabeth (Liz) Chirico who leads the Acquisition Innovation through Technology team in the Office of the Deputy Assistant Secretary of the Army (Procurement) (ODASA(P) and C</t>
   </si>
   <si>
     <t>Join the ACT-IAC IT Management and Modernization COI March 2023 meeting. Additional event information will be available soon.</t>
   </si>
   <si>
-    <t>The Voyager Class of 2023 invites all Fellows to Voyagers Got Talent showcasing the incredible talents of this year's Voyager Class. </t>
+    <t xml:space="preserve">The Voyager Class of 2023 invites all Fellows to Voyagers Got Talent showcasing the incredible talents of this year's Voyager Class. </t>
   </si>
   <si>
     <t>Join the ACT-IAC Cyber COI member meeting to hear from an invited government speakers Heather Kowalski, CIO, Interpol, Department of Justice, and Dr. Tiina KO Rodrigue, CISO, CFPB</t>
   </si>
   <si>
-    <t>This program is being planned by the Department of Education Federal Insights Exchange (FIE) planning team. </t>
+    <t xml:space="preserve">This program is being planned by the Department of Education Federal Insights Exchange (FIE) planning team. </t>
   </si>
   <si>
     <t>Join the ACT-IAC Evolving the Workforce COI March 2023 member meeting. More information about topic " The ABCs of Recruiting Gen Z" and speaker/s will be available soon.</t>
@@ -245,6 +238,9 @@
     <t>https://www.actiac.org/act-iac-event/federal-insights-exchange-featuring-dept-transportation-cio-cordell-schachter</t>
   </si>
   <si>
+    <t>TBD</t>
+  </si>
+  <si>
     <t>https://www.actiac.org/act-iac-event/climate-change-summit</t>
   </si>
   <si>
@@ -261,22 +257,13 @@
   </si>
   <si>
     <t>https://www.actiac.org/act-iac-event/imagine-nation-elc-2023</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,14 +313,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -380,7 +359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,27 +391,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,24 +425,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -657,16 +600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -706,7 +647,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -726,7 +667,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -746,7 +687,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -766,7 +707,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -786,7 +727,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -806,7 +747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -820,7 +761,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -840,7 +781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -860,7 +801,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -880,7 +821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -897,7 +838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -913,11 +854,11 @@
       <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -934,7 +875,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -950,8 +891,11 @@
       <c r="E15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -968,10 +912,10 @@
         <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -982,10 +926,10 @@
         <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1002,10 +946,10 @@
         <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1019,62 +963,29 @@
         <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F14" r:id="rId12"/>
+    <hyperlink ref="F15" r:id="rId13"/>
+    <hyperlink ref="F16" r:id="rId14"/>
+    <hyperlink ref="F17" r:id="rId15"/>
+    <hyperlink ref="F18" r:id="rId16"/>
+    <hyperlink ref="F19" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>